<commit_message>
Update Lab Diary and Results of Experiment 4
</commit_message>
<xml_diff>
--- a/hacking_the_simplespectro/experiments/Results_Blue53_Experiment_3.xlsx
+++ b/hacking_the_simplespectro/experiments/Results_Blue53_Experiment_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\simple-spectro\hacking_the_simplespectro\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E2D4C8-004D-49FC-88C4-97831D338CA3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5F6774-08B6-41CC-818A-2825AEA0722F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{1D5744FF-65D2-45FC-8D42-04693C4EBBF6}"/>
   </bookViews>
@@ -6741,8 +6741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65181045-6EB3-47C9-A473-A6EEB3DADC82}">
   <dimension ref="A1:AJ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>